<commit_message>
modify datasheet & generate rail sctipts
</commit_message>
<xml_diff>
--- a/camera_sequence.xlsx
+++ b/camera_sequence.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['C', 'D', 'A', 'B', 'C', 'B', 'D', 'A', 'C', 'D', 'A', 'B', 'B', 'D', 'A', 'C', 'D', 'B', 'C', 'A', 'D', 'C', 'B', 'A', 'C', 'B', 'A', 'D', 'B', 'C', 'A', 'D', 'C', 'B', 'A', 'D', 'C', 'D', 'A', 'B', 'A', 'C', 'D', 'B', 'A', 'D', 'C', 'B']</t>
+          <t>ABCDDCBACBADBDCAADBCCADBDABCCDBADBACABDCBCADDABC</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['C', 'D', 'A', 'B', 'C', 'B', 'D', 'A', 'C', 'D', 'A', 'B', 'B', 'D', 'A', 'C', 'D', 'B', 'C', 'A', 'D', 'C', 'B', 'A', 'C', 'B', 'A', 'D', 'B', 'C', 'A', 'D', 'C', 'B', 'A', 'D', 'C', 'D', 'A', 'B', 'A', 'C', 'D', 'B', 'A', 'D', 'C', 'B']</t>
+          <t>ABCDDCBACBADBDCAADBCCADBDABCCDBADBACABDCBCADDABC</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['D', 'C', 'B', 'A', 'C', 'D', 'A', 'B', 'C', 'D', 'A', 'B', 'B', 'A', 'C', 'D', 'B', 'A', 'C', 'D', 'A', 'B', 'C', 'D', 'C', 'D', 'B', 'A', 'D', 'C', 'B', 'A', 'B', 'A', 'C', 'D', 'A', 'D', 'C', 'B', 'D', 'B', 'A', 'C', 'D', 'C', 'B', 'A']</t>
+          <t>DABCABDCCBADDBCABCDABDACCABDDABCCBADCABDCDABBDAC</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['D', 'C', 'B', 'A', 'C', 'D', 'A', 'B', 'C', 'D', 'A', 'B', 'B', 'A', 'C', 'D', 'B', 'A', 'C', 'D', 'A', 'B', 'C', 'D', 'C', 'D', 'B', 'A', 'D', 'C', 'B', 'A', 'B', 'A', 'C', 'D', 'A', 'D', 'C', 'B', 'D', 'B', 'A', 'C', 'D', 'C', 'B', 'A']</t>
+          <t>DABCABDCCBADDBCABCDABDACCABDDABCCBADCABDCDABBDAC</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['B', 'C', 'A', 'D', 'C', 'D', 'A', 'B', 'B', 'D', 'C', 'A', 'C', 'A', 'D', 'B', 'D', 'A', 'C', 'B', 'A', 'D', 'B', 'C', 'C', 'B', 'A', 'D', 'A', 'D', 'B', 'C', 'D', 'B', 'C', 'A', 'D', 'C', 'A', 'B', 'C', 'B', 'D', 'A', 'A', 'B', 'D', 'C']</t>
+          <t>CBADACDBABDCBACDABDCBDACBDCADBACABDCCDBABCDABDAC</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['B', 'C', 'A', 'D', 'C', 'D', 'A', 'B', 'B', 'D', 'C', 'A', 'C', 'A', 'D', 'B', 'D', 'A', 'C', 'B', 'A', 'D', 'B', 'C', 'C', 'B', 'A', 'D', 'A', 'D', 'B', 'C', 'D', 'B', 'C', 'A', 'D', 'C', 'A', 'B', 'C', 'B', 'D', 'A', 'A', 'B', 'D', 'C']</t>
+          <t>CBADACDBABDCBACDABDCBDACBDCADBACABDCCDBABCDABDAC</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['D', 'C', 'B', 'A', 'A', 'B', 'C', 'D', 'A', 'D', 'B', 'C', 'C', 'A', 'B', 'D', 'C', 'B', 'A', 'D', 'A', 'D', 'B', 'C', 'D', 'B', 'C', 'A', 'A', 'D', 'B', 'C', 'A', 'D', 'B', 'C', 'B', 'A', 'C', 'D', 'D', 'A', 'B', 'C', 'B', 'C', 'D', 'A']</t>
+          <t>BDACABCDBCADACBDCDABDBCACABDADCBABDCBACDBCDADABC</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['D', 'C', 'B', 'A', 'A', 'B', 'C', 'D', 'A', 'D', 'B', 'C', 'C', 'A', 'B', 'D', 'C', 'B', 'A', 'D', 'A', 'D', 'B', 'C', 'D', 'B', 'C', 'A', 'A', 'D', 'B', 'C', 'A', 'D', 'B', 'C', 'B', 'A', 'C', 'D', 'D', 'A', 'B', 'C', 'B', 'C', 'D', 'A']</t>
+          <t>BDACABCDBCADACBDCDABDBCACABDADCBABDCBACDBCDADABC</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['B', 'C', 'D', 'A', 'D', 'A', 'B', 'C', 'A', 'D', 'C', 'B', 'C', 'A', 'B', 'D', 'A', 'C', 'B', 'D', 'B', 'D', 'C', 'A', 'A', 'C', 'B', 'D', 'A', 'B', 'C', 'D', 'D', 'B', 'A', 'C', 'C', 'B', 'D', 'A', 'B', 'C', 'D', 'A', 'D', 'C', 'A', 'B']</t>
+          <t>DBCACBDAACBDACDBDCABACDBADCBDABCDBACCDBAABCDADCB</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['B', 'C', 'D', 'A', 'D', 'A', 'B', 'C', 'A', 'D', 'C', 'B', 'C', 'A', 'B', 'D', 'A', 'C', 'B', 'D', 'B', 'D', 'C', 'A', 'A', 'C', 'B', 'D', 'A', 'B', 'C', 'D', 'D', 'B', 'A', 'C', 'C', 'B', 'D', 'A', 'B', 'C', 'D', 'A', 'D', 'C', 'A', 'B']</t>
+          <t>DBCACBDAACBDACDBDCABACDBADCBDABCDBACCDBAABCDADCB</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adapt to 5 cams perp rail set
</commit_message>
<xml_diff>
--- a/camera_sequence.xlsx
+++ b/camera_sequence.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,7 +469,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ADBCCABDACBDBCADBACDACBDCDABADBCCABDCDABADBCBADCCBADABCDACDBADCBACBDADCBACBDBCDAACDBADBCBCADBACDDABCDBACCABDBCDABDACADCBCADBDABCABCDADCBBADCDCBADACBBACDBCDABDACCDBACDBADBCADCABDCABDACBCADBDABCACBDCADBACBDBDACBADCBCDABADCBDACADCBCDABCBADADCBDBACBDCABDCADCABDCABACDBACDBCADBDBACCADBBACDACDBCABDDACBABDCACDBABDCDACBDCABDCABBACDDABCADCBADCBBDCABADCADBCBCDABDCADCABDBCADACBDCABDCBADABCBCADCDABADCBACDBBCDACBDADBCABADCADCBADCBBDACABCDACDBBCDADACBBCDADACBCBDABDCAABDCACDBDCABCDBABACDBADCCDABADBCBCDAADBCABDCADCBBCADBADCCADBBCADABDCDBCAACDBADCBADBCCBDAABDCDBCADBACBACDCABDBACDACBDADCBABDCDABCDCABCBADCBDABDCADCBABCADBADCBCADDCBACBADDBCADABCABDCCABDACDBADCBBDCAACBDBDACDACBABDCADCBADCBCDABCDBAACDBBDCADCBACDBAADBCBADCBCADDABCCDBAABCDDACBCDABDCABDBACABCDCBDABADCABDCBACDACBDCDBABACDBDCADABCBADCADCBADCBCDBADCAB</t>
+          <t>DCEABBACEDDECABEABDCCAEDBCAEDBBDACEBECADEADCBADEBCABCEDCDAEBEBCADDCAEBAEDBCCBEADADEBCCDEABDECBAECBDAEDCABEABCDBECADAEDBCDABECDECBAABCDEADECBBEACDAEBDCEDBACECABDBADECEACBDEDBACDCEBAABEDCDCBEACEADBEBDACAEDBCBEACDEACBDCBDAEBECDAEBADCADBECADCBEBDCAEBECDACBEADECABDCDBAEACDBEECADBDBECACEDABABDCEDEBACDABCECABDEBCEDADECBACEDABBDCAECABEDCABEDECADBCADEBDBCAEECDBAEABCDCDEABADCEBBEADCBDACEEDACBEDABCBAECDCDEBADEBCAEDCBACEADBDAEBCEDBACCAEDBECBADACBDECADEBBEACDBAEDCBCDAEEBACDABCDEEDBACBAECDBDCEAACBEDBECADECADBBAEDCADECBECDABCBEADDECABBAECDCABDEEDBACCDBAEDBCEACEDBADAECBBEADCEABCDDBCAEEBDCAACEDBCBDAEBCDEADECABBADECEBDCAACDBEAEBCDDCAEBABCDEABEDCEDBCAEDCABCBEDADEACBDCAEBAECDBCEDBADEACBEACBDBDACEACEBDDEBCABEADCEACBDECABDCBDEACADBEABCEDEDCBAADECBABCEDEBDACECDABDCEBAEDCABACDEBEBDCAAEBDCCBADEADBECBADECAEDBCBCAEDDCAEBCADEBDBEACCBAEDABDCEDBAECCABDECEADBCAEBDABECDDACEBEDACBDBECADABECECBDABDECACBAEDEDABCECBDAADECBCDBEAADECBCEBDABEDACBCEDACAEBDCEABDCDEABCDAEBCDABECBDAECABEDCBEDADEBCACEBADCADEBACBDEECDABDEBACEADCBCBADEEDCBACEBADEDABCADBCEDCEABEDBCAECDBAABDCEEADCBDCABEBDEACDACBEEACDBBDCEACDEBACADBEEABCDACEDBCBAEDCBAEDCBAEDECBDABEDCACEBDAABCDEEBCADDBCAECDBAEEDCBADEABCDBAECEACDBEACBDBDECAECADBDCAEBADBCECABEDBDACECEABDEDACBACBDEDBECACEBDAECDBAACDBEEBDACECBADDEABCCBAEDABCDE</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ADBCCABDACBDBCADBACDACBDCDABADBCCABDCDABADBCBADCCBADABCDACDBADCBACBDADCBACBDBCDAACDBADBCBCADBACDDABCDBACCABDBCDABDACADCBCADBDABCABCDADCBBADCDCBADACBBACDBCDABDACCDBACDBADBCADCABDCABDACBCADBDABCACBDCADBACBDBDACBADCBCDABADCBDACADCBCDABCBADADCBDBACBDCABDCADCABDCABACDBACDBCADBDBACCADBBACDACDBCABDDACBABDCACDBABDCDACBDCABDCABBACDDABCADCBADCBBDCABADCADBCBCDABDCADCABDBCADACBDCABDCBADABCBCADCDABADCBACDBBCDACBDADBCABADCADCBADCBBDACABCDACDBBCDADACBBCDADACBCBDABDCAABDCACDBDCABCDBABACDBADCCDABADBCBCDAADBCABDCADCBBCADBADCCADBBCADABDCDBCAACDBADCBADBCCBDAABDCDBCADBACBACDCABDBACDACBDADCBABDCDABCDCABCBADCBDABDCADCBABCADBADCBCADDCBACBADDBCADABCABDCCABDACDBADCBBDCAACBDBDACDACBABDCADCBADCBCDABCDBAACDBBDCADCBACDBAADBCBADCBCADDABCCDBAABCDDACBCDABDCABDBACABCDCBDABADCABDCBACDACBDCDBABACDBDCADABCBADCADCBADCBCDBADCAB</t>
+          <t>DCEABBACEDDECABEABDCCAEDBCAEDBBDACEBECADEADCBADEBCABCEDCDAEBEBCADDCAEBAEDBCCBEADADEBCCDEABDECBAECBDAEDCABEABCDBECADAEDBCDABECDECBAABCDEADECBBEACDAEBDCEDBACECABDBADECEACBDEDBACDCEBAABEDCDCBEACEADBEBDACAEDBCBEACDEACBDCBDAEBECDAEBADCADBECADCBEBDCAEBECDACBEADECABDCDBAEACDBEECADBDBECACEDABABDCEDEBACDABCECABDEBCEDADECBACEDABBDCAECABEDCABEDECADBCADEBDBCAEECDBAEABCDCDEABADCEBBEADCBDACEEDACBEDABCBAECDCDEBADEBCAEDCBACEADBDAEBCEDBACCAEDBECBADACBDECADEBBEACDBAEDCBCDAEEBACDABCDEEDBACBAECDBDCEAACBEDBECADECADBBAEDCADECBECDABCBEADDECABBAECDCABDEEDBACCDBAEDBCEACEDBADAECBBEADCEABCDDBCAEEBDCAACEDBCBDAEBCDEADECABBADECEBDCAACDBEAEBCDDCAEBABCDEABEDCEDBCAEDCABCBEDADEACBDCAEBAECDBCEDBADEACBEACBDBDACEACEBDDEBCABEADCEACBDECABDCBDEACADBEABCEDEDCBAADECBABCEDEBDACECDABDCEBAEDCABACDEBEBDCAAEBDCCBADEADBECBADECAEDBCBCAEDDCAEBCADEBDBEACCBAEDABDCEDBAECCABDECEADBCAEBDABECDDACEBEDACBDBECADABECECBDABDECACBAEDEDABCECBDAADECBCDBEAADECBCEBDABEDACBCEDACAEBDCEABDCDEABCDAEBCDABECBDAECABEDCBEDADEBCACEBADCADEBACBDEECDABDEBACEADCBCBADEEDCBACEBADEDABCADBCEDCEABEDBCAECDBAABDCEEADCBDCABEBDEACDACBEEACDBBDCEACDEBACADBEEABCDACEDBCBAEDCBAEDCBAEDECBDABEDCACEBDAABCDEEBCADDBCAECDBAEEDCBADEABCDBAECEACDBEACBDBDECAECADBDCAEBADBCECABEDBDACECEABDEDACBACBDEDBECACEBDAECDBAACDBEEBDACECBADDEABCCBAEDABCDE</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CDABCBDADCBACABDBACDABCDCBDADCBACDABBCADBADCACDBCABDCABDCBDABCDADBACBDCABADCACDBBCDABACDACBDADCBACDBCBADDBACCDBADBACBADCABDCADBCDCBABCDABCDACABDABCDABDCACBDBCDABCADCADBBDCAABDCDABCDABCCABDBDCABACDCDABBCADBACDABCDADCBBDCACADBABCDCDABBADCDCBAABDCCADBBDACBACDBDCAADCBCABDCDABACDBDCBACDABCDABBDACBACDACDBCDABCBADDBACDACBDABCABCDDACBBDACABDCBDCADACBCBADBDACDBCAABDCCBADBDCAABDCABCDACBDCADBBDACABDCABDCADCBACDBCDBAADCBCBDACBDABACDCADBCDBABCADBCADBADCBACDADBCBACDDACBBCADCADBDABCDABCCDBACBADBDCABACDCBDADCABABCDACDBBADCBDCAADCBDABCACDBCABDCDBAABCDCDABCBDABACDDBACCDBACDBADABCCABDCDABDCBAABCDACDBBCDABADCABCDCBDABCDABCADBACDDBCABDCADABCCABDABDCBDACABDCCABDDACBCBADCABDACDBADBCCADBDCBABCDACDABABCDBDCACBADDCBABDACCBDACBADBADCADCBCABDBCDADACBDCABDBACCADBADCBDCABBDACCBADCDBABACDDCBABDACADCBABCDDABCCBADABDCBDAC</t>
+          <t>BDCEACDEBAAEDCBEDABCEBACDCABEDBECADBACEDAECDBDEBACABCDEACEDBDABECBADECECABDBADCEBDACEAEBDCDACBEDCBAEDECBAAECDBCEBADCABDECDBEAABECDEADCBEDCABEBDCACEABDECDABBADECBDEACEADCBECADBADCEBADBCEBCAEDBCADECAEDBAECBDCADEBADEBCDACEBBDAECBCADEDACBEDBCEADCAEBECDBAAECBDECDABDCEABECABDAEBDCACBEDABEDCADBECDBEACADECBDABCEDBCEAEBCADABEDCBACDEBEDACBDEACBDEACCADEBBCAEDEACDBBDECACADEBBADCEDBECAACEBDACEDBBECADADCBEAEBDCECABDCEABDECBADCDBAEAEDCBABCEDACBEDCEBDADABECDCABECADBEDECABBDAECEDABCCDAEBDEBACDCEBAEBDACCDABEDCEABBACEDDEACBABEDCEDBACDECBACDAEBDABECDACBEECADBADECBDCBEADCEABAEDCBEABCDEBADCACBEDAECDBDEBACEDCBADBECAECADBCEDBADABECDECABCDBAEDCAEBAECDBCADBEBCEDACAEBDAEBCDCBDAECEABDEBDACAECDBBDCEABDCEADCEBAACDEBDEBCAADEBCADBCEDBECABCAEDAEDCBACDBEAECBDBADECCDBEABDACEACDBEBCADEBCAEDDACBECBDEACAEBDBAECDEDABCCEBDAEBACDCADEBBCEDAEACBDABCDEBECDAACDBECDBEABAEDCDCAEBADBCEADEBCBCADECDBAEAEBDCCEDABECADBCBDEABAEDCBCEDABDEACDACBEBADCECBADEBACDEEBADCCBEDAAECDBEDBACBADECDEBCAECDABBDCEACDEBACDEBAEBCDAABEDCDBCEAEACDBBACEDADBCEEBADCEACBDAEBDCAEDBCCEDABADEBCECBDACAEBDCEBDAADBECBCEADBDECAEBDACEBDCAECABDBDCEACEDABADCBEDACEBADBCECDEABEBACDEACBDEBDACBDECAEDCBAACDEBCBAEDABCDEECBADEABCDECBADDEBCAABDECEDACBADBCECEBADADCBECBDAEECABDEDCBADEBCABECADAEBDCCEDABABDECEABDCACDBEDCEABDCBEADABCECABDE</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CDABCBDADCBACABDBACDABCDCBDADCBACDABBCADBADCACDBCABDCABDCBDABCDADBACBDCABADCACDBBCDABACDACBDADCBACDBCBADDBACCDBADBACBADCABDCADBCDCBABCDABCDACABDABCDABDCACBDBCDABCADCADBBDCAABDCDABCDABCCABDBDCABACDCDABBCADBACDABCDADCBBDCACADBABCDCDABBADCDCBAABDCCADBBDACBACDBDCAADCBCABDCDABACDBDCBACDABCDABBDACBACDACDBCDABCBADDBACDACBDABCABCDDACBBDACABDCBDCADACBCBADBDACDBCAABDCCBADBDCAABDCABCDACBDCADBBDACABDCABDCADCBACDBCDBAADCBCBDACBDABACDCADBCDBABCADBCADBADCBACDADBCBACDDACBBCADCADBDABCDABCCDBACBADBDCABACDCBDADCABABCDACDBBADCBDCAADCBDABCACDBCABDCDBAABCDCDABCBDABACDDBACCDBACDBADABCCABDCDABDCBAABCDACDBBCDABADCABCDCBDABCDABCADBACDDBCABDCADABCCABDABDCBDACABDCCABDDACBCBADCABDACDBADBCCADBDCBABCDACDABABCDBDCACBADDCBABDACCBDACBADBADCADCBCABDBCDADACBDCABDBACCADBADCBDCABBDACCBADCDBABACDDCBABDACADCBABCDDABCCBADABDCBDAC</t>
+          <t>BDCEACDEBAAEDCBEDABCEBACDCABEDBECADBACEDAECDBDEBACABCDEACEDBDABECBADECECABDBADCEBDACEAEBDCDACBEDCBAEDECBAAECDBCEBADCABDECDBEAABECDEADCBEDCABEBDCACEABDECDABBADECBDEACEADCBECADBADCEBADBCEBCAEDBCADECAEDBAECBDCADEBADEBCDACEBBDAECBCADEDACBEDBCEADCAEBECDBAAECBDECDABDCEABECABDAEBDCACBEDABEDCADBECDBEACADECBDABCEDBCEAEBCADABEDCBACDEBEDACBDEACBDEACCADEBBCAEDEACDBBDECACADEBBADCEDBECAACEBDACEDBBECADADCBEAEBDCECABDCEABDECBADCDBAEAEDCBABCEDACBEDCEBDADABECDCABECADBEDECABBDAECEDABCCDAEBDEBACDCEBAEBDACCDABEDCEABBACEDDEACBABEDCEDBACDECBACDAEBDABECDACBEECADBADECBDCBEADCEABAEDCBEABCDEBADCACBEDAECDBDEBACEDCBADBECAECADBCEDBADABECDECABCDBAEDCAEBAECDBCADBEBCEDACAEBDAEBCDCBDAECEABDEBDACAECDBBDCEABDCEADCEBAACDEBDEBCAADEBCADBCEDBECABCAEDAEDCBACDBEAECBDBADECCDBEABDACEACDBEBCADEBCAEDDACBECBDEACAEBDBAECDEDABCCEBDAEBACDCADEBBCEDAEACBDABCDEBECDAACDBECDBEABAEDCDCAEBADBCEADEBCBCADECDBAEAEBDCCEDABECADBCBDEABAEDCBCEDABDEACDACBEBADCECBADEBACDEEBADCCBEDAAECDBEDBACBADECDEBCAECDABBDCEACDEBACDEBAEBCDAABEDCDBCEAEACDBBACEDADBCEEBADCEACBDAEBDCAEDBCCEDABADEBCECBDACAEBDCEBDAADBECBCEADBDECAEBDACEBDCAECABDBDCEACEDABADCBEDACEBADBCECDEABEBACDEACBDEBDACBDECAEDCBAACDEBCBAEDABCDEECBADEABCDECBADDEBCAABDECEDACBADBCECEBADADCBECBDAEECABDEDCBADEBCABECADAEBDCCEDABABDECEABDCACDBEDCEABDCBEADABCECABDE</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DCABABCDBCADADCBADCBCDABBCADBCADBDCAADCBACBDADBCADCBACDBDCBAACDBBCDADBCADCABDCABBADCCADBABDCBDCADCABBCDACBDACBDABCADCBDAADCBDCABABCDCDBADABCADBCBCDADABCDBCACDBACBDAABDCDCBADBCACDBADCABCBADBADCBACDDBCADCABDACBDCBAABCDCBDABADCACBDCABDABCDBCADBDACABCDBADCABDCCDBAACDBDBCACBDABCADCBADABCDBCDACABDADBCDBACBACDDBACDBACDBCABCDABADCDBACBADCABDCDBACCDBABDCABDCAADBCBACDABCDDABCABCDABCDBACDDACBDACBDACBBDACDCBABADCBADCCABDDACBADCBBDACCABDBADCABDCACDBACDBBADCDCBABCDABADCABCDDABCBADCADBCACBDDBCAADCBCDBAADBCDACBBDACABDCABCDABCDABCDBDCADABCCBADDACBCDABCDABDBACADBCADBCDACBABDCCADBBADCADBCABCDBCADDCABDBACDCABDBACBCADACDBDBACABDCABCDCBDABCADBCDADACBBDCADBACCBADBDACBACDDCABDABCDBCADBCABACDCDBADBACDABCBADCDBACDBCAABCDDACBABDCBDCADCABADBCDCBABDACACDBACBDADCBBCADDCBABADCCBADCBADCABDACBDADBCACDBCDABCDBACADBCDBADABC</t>
+          <t>EABDCDEBCAEADBCEDCBACDBEADBCEACBEADBCDEACEADBABDCEECDABEDACBACEBDDAECBEBADCEACBDBCAEDABDCEBCDEAEBDACDCEABABEDCCAEBDDBCEAAECBDCBADEDECBAABDECEABDCCAEDBADBCEEADCBBCEADDCBEABECADEACBDEDABCACEDBCABDECBDAEAECDBCAEBDEBCDAACDEBDBCAEAEBCDEDCBAACEBDCBADEBAEDCECDBADEBCAEABCDAEBCDACBEDACBDECEDABEBACDBEACDACDBEBAEDCBDCAECEBADDBECADACEBDCEBAADEBCCEBDACBADECEDBABCAEDDAECBEADBCCDEBADBCEAADBCEAEDBCBEDCACEDBACDBAECAEBDDACBEBDCAEADBECCBEADCBEDABDAECBCEADBCEDABCDAECADBEEABCDDEBACABEDCAEDCBDAECBCBEADCABDECADBEEADCBEBACDEBCADBCEADABECDCEDBABDACEDBCEAEDABCEACDBBCEADDCBEACEDBAACDBEADBECADCEBBEDACACEBDBDECAABCDEDBCAEBDEACBACDECBDEAEBCADDCEBAADCEBABCEDBAEDCBDEACEBADCBCDEACEABDEADBCCDBAEADECBCADBECDEBADACBEEDCABCDEABCAEDBEBADCECBDAECDABDCEBADCBAEEBADCECADBBCDAEBACEDDEABCCDBEADCBEAADECBAEDCBCEDABEADCBDBAECCDABEEADCBDCEBACDAEBCAEDBBCADEBAECDCAEDBABEDCDACBEBDAECECBDAECADBAECBDDBECADCBEAACDBEDBCAEDAECBEABCDABECDDACEBBCDAECDAEBCAEBDABDCEBACDEDBACEBDACECEDABCEADBABEDCCBADEAECDBDAEBCDCAEBDAECBDCAEBDCABECABDEEADCBECABDCABEDDEBCAADECBBCDAEACEDBCDBEAAEDCBECADBDBEACEACBDADEBCCEBADBAECDCADEBABECDCDEBAABCDEECBDAAEDBCCABEDDBAECACDBEADCBECBEDADAECBAEDCBADCEBAEBDCCABDEACBEDEDCABECDABBDECACADEBCAEBDBDECAADCBEABCEDBDCEAACDBEABCEDACBDECADEBCEDABDABECEDABCBACEDBCDAEBCEADCDBEAEABDCCEDBA</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DCABABCDBCADADCBADCBCDABBCADBCADBDCAADCBACBDADBCADCBACDBDCBAACDBBCDADBCADCABDCABBADCCADBABDCBDCADCABBCDACBDACBDABCADCBDAADCBDCABABCDCDBADABCADBCBCDADABCDBCACDBACBDAABDCDCBADBCACDBADCABCBADBADCBACDDBCADCABDACBDCBAABCDCBDABADCACBDCABDABCDBCADBDACABCDBADCABDCCDBAACDBDBCACBDABCADCBADABCDBCDACABDADBCDBACBACDDBACDBACDBCABCDABADCDBACBADCABDCDBACCDBABDCABDCAADBCBACDABCDDABCABCDABCDBACDDACBDACBDACBBDACDCBABADCBADCCABDDACBADCBBDACCABDBADCABDCACDBACDBBADCDCBABCDABADCABCDDABCBADCADBCACBDDBCAADCBCDBAADBCDACBBDACABDCABCDABCDABCDBDCADABCCBADDACBCDABCDABDBACADBCADBCDACBABDCCADBBADCADBCABCDBCADDCABDBACDCABDBACBCADACDBDBACABDCABCDCBDABCADBCDADACBBDCADBACCBADBDACBACDDCABDABCDBCADBCABACDCDBADBACDABCBADCDBACDBCAABCDDACBABDCBDCADCABADBCDCBABDACACDBACBDADCBBCADDCBABADCCBADCBADCABDACBDADBCACDBCDABCDBACADBCDBADABC</t>
+          <t>EABDCDEBCAEADBCEDCBACDBEADBCEACBEADBCDEACEADBABDCEECDABEDACBACEBDDAECBEBADCEACBDBCAEDABDCEBCDEAEBDACDCEABABEDCCAEBDDBCEAAECBDCBADEDECBAABDECEABDCCAEDBADBCEEADCBBCEADDCBEABECADEACBDEDABCACEDBCABDECBDAEAECDBCAEBDEBCDAACDEBDBCAEAEBCDEDCBAACEBDCBADEBAEDCECDBADEBCAEABCDAEBCDACBEDACBDECEDABEBACDBEACDACDBEBAEDCBDCAECEBADDBECADACEBDCEBAADEBCCEBDACBADECEDBABCAEDDAECBEADBCCDEBADBCEAADBCEAEDBCBEDCACEDBACDBAECAEBDDACBEBDCAEADBECCBEADCBEDABDAECBCEADBCEDABCDAECADBEEABCDDEBACABEDCAEDCBDAECBCBEADCABDECADBEEADCBEBACDEBCADBCEADABECDCEDBABDACEDBCEAEDABCEACDBBCEADDCBEACEDBAACDBEADBECADCEBBEDACACEBDBDECAABCDEDBCAEBDEACBACDECBDEAEBCADDCEBAADCEBABCEDBAEDCBDEACEBADCBCDEACEABDEADBCCDBAEADECBCADBECDEBADACBEEDCABCDEABCAEDBEBADCECBDAECDABDCEBADCBAEEBADCECADBBCDAEBACEDDEABCCDBEADCBEAADECBAEDCBCEDABEADCBDBAECCDABEEADCBDCEBACDAEBCAEDBBCADEBAECDCAEDBABEDCDACBEBDAECECBDAECADBAECBDDBECADCBEAACDBEDBCAEDAECBEABCDABECDDACEBBCDAECDAEBCAEBDABDCEBACDEDBACEBDACECEDABCEADBABEDCCBADEAECDBDAEBCDCAEBDAECBDCAEBDCABECABDEEADCBECABDCABEDDEBCAADECBBCDAEACEDBCDBEAAEDCBECADBDBEACEACBDADEBCCEBADBAECDCADEBABECDCDEBAABCDEECBDAAEDBCCABEDDBAECACDBEADCBECBEDADAECBAEDCBADCEBAEBDCCABDEACBEDEDCABECDABBDECACADEBCAEBDBDECAADCBEABCEDBDCEAACDBEABCEDACBDECADEBCEDABDABECEDABCBACEDBCDAEBCEADCDBEAEABDCCEDBA</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ADBCBACDDCBAACDBADBCBCADCABDCADBBACDBDACDACBCDABBCDADABCCDBADCABACBDACBDCBDACBADACDBBADCDBCABACDCBDAADBCCDBABACDCBDACDBABDCABDACADBCDCABBADCBACDDABCDACBDCBABACDCADBBACDBDCACBADDACBCADBBDACDACBDACBDACBABCDDBCAADCBDABCBDACDCBADABCDBACDBCADBACBACDDCBADACBDCABADBCBACDBACDBCADDACBADBCBCADCABDADCBCADBACBDDCBADBACCABDBADCADCBACDBADBCADCBDBCAABCDADCBBDACBCDABACDDCBAACDBBCDAADCBBDACDBCADCBABACDCADBBCADDCBABDCAABCDABDCDCBAADCBABDCBDCADACBADBCACBDABCDBADCDBCABDCABCDADCABDACBABDCDBACDCBAACDBCDBADABCDACBCABDBADCADCBBDACCABDCDABDBACABDCDABCACDBBADCADCBDABCABDCDBCACADBDACBBCADBCADCBDABCADDCABCADBBCDACABDABDCDBACABDCDBACADCBABCDACBDCBDADCBAABDCBCDAADBCACDBBADCADBCACBDCBADABDCACBDABDCCBDACBADCADBDBACBDACADCBCABDCBDACBDABDCABCADCDABDBCAABCDBDACDCBADABCDBCACBADCBDABADCABDCDABCDABCDABCACBDCBDAABCDACDBBDCABACD</t>
+          <t>DBECAEBDCADCEBAAECBDADEBCDECABCBAEDEABCDBDECADEACBDECABDABECADCBEEABCDCDBAEDCEBAAECDBDCBEACADBEBCDEADECABCDEBADCEBACEBDABACDEECABDEADBCECDABECBDACADEBBEDCAEDBCAABDCECDBEABACDEBCEDACADEBDACBECADBEBEADCCEBADCADEBACBEDADEBCEADBCEBADCCBDEACABDEDEBACCADEBEDBACBACDEDEABCDABCEDEABCDAECBDBAECCADEBAECBDBDACEBAEDCEDACBDABECCADBEBDEACBADECEBCDAABDECBADCEDECABDABECBACEDBCDEAECADBDCEABCBAEDBECDACEADBEABDCAEBCDDEBACBCEDACEADBBDCAEEACBDDBACEAECBDBAEDCCEADBBCADEEABDCCABEDEBDCADEABCEADCBADEBCEACDBDCABEDEBACEBCADAECBDABECDDBACEABDECEBACDCEBADEADCBBECDABAECDDABECEABCDDBACEEACBDBEADCDCBEAECADBBCAEDDABECEBACDDCEBADCBAEDCAEBBDACEEADBCCBDAEBADECCAEBDDCEABBCDEABCEADADBECEBADCCBEADAEBCDEDACBAEDCBBEADCCAEBDDECBAEDCABCBEADEDACBBADCECABDEDECABCBEDAEACDBADECBCBADEDABCECBAEDAECBDCADBEADCEBDEBACACBDEEABCDBDECADBAECDABECDAECBBAEDCDBACEDCEBAABDECBDEACDBAECADCEBEBDCABCDAEADEBCDEABCAEDBCEDBCABCDAECDABECEDABCEADBADCEBEDCBADACBECBAEDEDCBAABEDCEACDBCEBDABEDACCAEDBBEDACADBCECABEDBEADCACDBECBEADCBDAEEDBCAEBDACEDBCAEBDCACBEADBADCECBDAECDEABAEDBCBACEDDECBABEDACDABECAECBDBCADEDBACEABECDADECBCBEADCBDEAEDBCABDCEADABECEDBACDEBACDEABCECDABADEBCBEACDADCEBEACBDDEBACACBDECBADEEACDBDEBACBCAEDEDCABBADCEDACEBAECBDCADEBDEABCDBAECACEBDBDCAEAEDCBCEDBACBADEEADCBBEACDBDECAEDACBACDBEEDABCDECABADBCE</t>
         </is>
       </c>
     </row>
@@ -595,43 +595,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ADBCBACDDCBAACDBADBCBCADCABDCADBBACDBDACDACBCDABBCDADABCCDBADCABACBDACBDCBDACBADACDBBADCDBCABACDCBDAADBCCDBABACDCBDACDBABDCABDACADBCDCABBADCBACDDABCDACBDCBABACDCADBBACDBDCACBADDACBCADBBDACDACBDACBDACBABCDDBCAADCBDABCBDACDCBADABCDBACDBCADBACBACDDCBADACBDCABADBCBACDBACDBCADDACBADBCBCADCABDADCBCADBACBDDCBADBACCABDBADCADCBACDBADBCADCBDBCAABCDADCBBDACBCDABACDDCBAACDBBCDAADCBBDACDBCADCBABACDCADBBCADDCBABDCAABCDABDCDCBAADCBABDCBDCADACBADBCACBDABCDBADCDBCABDCABCDADCABDACBABDCDBACDCBAACDBCDBADABCDACBCABDBADCADCBBDACCABDCDABDBACABDCDABCACDBBADCADCBDABCABDCDBCACADBDACBBCADBCADCBDABCADDCABCADBBCDACABDABDCDBACABDCDBACADCBABCDACBDCBDADCBAABDCBCDAADBCACDBBADCADBCACBDCBADABDCACBDABDCCBDACBADCADBDBACBDACADCBCABDCBDACBDABDCABCADCDABDBCAABCDBDACDCBADABCDBCACBADCBDABADCABDCDABCDABCDABCACBDCBDAABCDACDBBDCABACD</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>acSn042190120031</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>CABDBCADCDABDBCAADBCADCBBCDACADBACDBDBACABDCCABDBACDDCBACADBDABCDCBACDBADBACADCBDBACBCADBCADCADBDBCAABDCBDACADCBACDBDCABABDCDABCBDCABCDACADBDCBADBACCDBADACBBDACBDCAADBCADCBDBCADCABCADBDCABDACBADBCBACDDBACCADBACDBCABDCBADCADBDBACCBDAACBDACDBACBDDCABBADCCBDACBADABDCDBACDCBAADBCBACDCDABCDABACBDBDACBACDDBACBCADCADBBACDBCADCABDBACDCABDBCADCBDACDBADCABCABDDCABACDBDBACADBCBDACBCDAADBCABCDACBDCDABBADCBCADBADCCDBACDABCDBABDACBACDADBCDCBAACDBDACBCBDACBDACDBAABDCBADCABCDBDACDABCABCDACDBCADBCDABCBDACBADADBCDACBACBDCBADDBCADBCABADCADCBACBDACDBDABCCDBACBADDCBAABDCCDBAABDCACDBCDBADACBDABCCDABDACBBADCBDCAADBCADCBBADCADCBABDCBDCACABDBACDCADBABDCBDACBACDABDCCDABDBCADCBAABCDADBCCBDABACDBACDDCABDCBAACDBBACDCDBADACBDCABADBCCDABDCABBADCACDBDACBCBADDCABDBCAADBCBACDBCADDBACCBDACDABDCBAABDCCDBACDBADABCDBACACBDCADB</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>acSn042051920077</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>CABDBCADCDABDBCAADBCADCBBCDACADBACDBDBACABDCCABDBACDDCBACADBDABCDCBACDBADBACADCBDBACBCADBCADCADBDBCAABDCBDACADCBACDBDCABABDCDABCBDCABCDACADBDCBADBACCDBADACBBDACBDCAADBCADCBDBCADCABCADBDCABDACBADBCBACDDBACCADBACDBCABDCBADCADBDBACCBDAACBDACDBACBDDCABBADCCBDACBADABDCDBACDCBAADBCBACDCDABCDABACBDBDACBACDDBACBCADCADBBACDBCADCABDBACDCABDBCADCBDACDBADCABCABDDCABACDBDBACADBCBDACBCDAADBCABCDACBDCDABBADCBCADBADCCDBACDABCDBABDACBACDADBCDCBAACDBDACBCBDACBDACDBAABDCBADCABCDBDACDABCABCDACDBCADBCDABCBDACBADADBCDACBACBDCBADDBCADBCABADCADCBACBDACDBDABCCDBACBADDCBAABDCCDBAABDCACDBCDBADACBDABCCDABDACBBADCBDCAADBCADCBBADCADCBABDCBDCACABDBACDCADBABDCBDACBACDABDCCDABDBCADCBAABCDADBCCBDABACDBACDDCABDCBAACDBBACDCDBADACBDCABADBCCDABDCABBADCACDBDACBCBADDCABDBCAADBCBACDBCADDBACCBDACDABDCBAABDCCDBACDBADABCDBACACBDCADB</t>
+          <t>DBECAEBDCADCEBAAECBDADEBCDECABCBAEDEABCDBDECADEACBDECABDABECADCBEEABCDCDBAEDCEBAAECDBDCBEACADBEBCDEADECABCDEBADCEBACEBDABACDEECABDEADBCECDABECBDACADEBBEDCAEDBCAABDCECDBEABACDEBCEDACADEBDACBECADBEBEADCCEBADCADEBACBEDADEBCEADBCEBADCCBDEACABDEDEBACCADEBEDBACBACDEDEABCDABCEDEABCDAECBDBAECCADEBAECBDBDACEBAEDCEDACBDABECCADBEBDEACBADECEBCDAABDECBADCEDECABDABECBACEDBCDEAECADBDCEABCBAEDBECDACEADBEABDCAEBCDDEBACBCEDACEADBBDCAEEACBDDBACEAECBDBAEDCCEADBBCADEEABDCCABEDEBDCADEABCEADCBADEBCEACDBDCABEDEBACEBCADAECBDABECDDBACEABDECEBACDCEBADEADCBBECDABAECDDABECEABCDDBACEEACBDBEADCDCBEAECADBBCAEDDABECEBACDDCEBADCBAEDCAEBBDACEEADBCCBDAEBADECCAEBDDCEABBCDEABCEADADBECEBADCCBEADAEBCDEDACBAEDCBBEADCCAEBDDECBAEDCABCBEADEDACBBADCECABDEDECABCBEDAEACDBADECBCBADEDABCECBAEDAECBDCADBEADCEBDEBACACBDEEABCDBDECADBAECDABECDAECBBAEDCDBACEDCEBAABDECBDEACDBAECADCEBEBDCABCDAEADEBCDEABCAEDBCEDBCABCDAECDABECEDABCEADBADCEBEDCBADACBECBAEDEDCBAABEDCEACDBCEBDABEDACCAEDBBEDACADBCECABEDBEADCACDBECBEADCBDAEEDBCAEBDACEDBCAEBDCACBEADBADCECBDAECDEABAEDBCBACEDDECBABEDACDABECAECBDBCADEDBACEABECDADECBCBEADCBDEAEDBCABDCEADABECEDBACDEBACDEABCECDABADEBCBEACDADCEBEACBDDEBACACBDECBADEEACDBDEBACBCAEDEDCABBADCEDACEBAECBDCADEBDEABCDBAECACEBDBDCAEAEDCBCEDBACBADEEADCBBEACDBDECAEDACBACDBEEDABCDECABADBCE</t>
         </is>
       </c>
     </row>

</xml_diff>